<commit_message>
Comitting all changed files. Most imp changes are in NseOptionChain.py
</commit_message>
<xml_diff>
--- a/Excels/IntradayTrend.xlsx
+++ b/Excels/IntradayTrend.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>S.No</t>
+  </si>
+  <si>
+    <t>NIFTY</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>ALL</t>
   </si>
 </sst>
 </file>
@@ -212,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -227,16 +239,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -293,36 +339,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -337,12 +353,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:E26" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:E26" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="4">
-    <tableColumn id="5" name="S.No" dataDxfId="8"/>
+    <tableColumn id="5" name="S.No" dataDxfId="4"/>
     <tableColumn id="2" name="Bullish"/>
     <tableColumn id="3" name="Bearish"/>
-    <tableColumn id="4" name="Diff" dataDxfId="11">
+    <tableColumn id="4" name="Diff" dataDxfId="3">
       <calculatedColumnFormula>(C6-D6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -351,20 +367,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="G5:K26" totalsRowShown="0">
-  <autoFilter ref="G5:K26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="G5:L26" totalsRowShown="0">
+  <autoFilter ref="G5:L26">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
-    <tableColumn id="2" name="Diff" dataDxfId="10"/>
+  <tableColumns count="6">
+    <tableColumn id="2" name="Diff" dataDxfId="2"/>
     <tableColumn id="3" name="Bullish"/>
     <tableColumn id="4" name="Bearish"/>
     <tableColumn id="5" name="NF Close"/>
-    <tableColumn id="6" name="↑/↓" dataDxfId="9"/>
+    <tableColumn id="6" name="↑/↓" dataDxfId="1"/>
+    <tableColumn id="1" name="DATA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -667,10 +684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U74"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,26 +710,26 @@
     <col min="18" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="P2" s="12" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="P2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="12"/>
+      <c r="Q2" s="14"/>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C3" s="13" t="s">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="G3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
       <c r="L3"/>
       <c r="N3" t="s">
         <v>14</v>
@@ -721,9 +739,9 @@
       </c>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="J4" s="10">
-        <v>22605</v>
+        <v>22404</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4"/>
@@ -732,7 +750,7 @@
       </c>
       <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>34</v>
       </c>
@@ -760,7 +778,9 @@
       <c r="K5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L5"/>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
       <c r="M5" s="6" t="s">
         <v>0</v>
       </c>
@@ -788,154 +808,164 @@
       <c r="U5" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+      <c r="V5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E26" si="0">(C6-D6)</f>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ref="G6:G26" si="1">H6-I6</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I6">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="J6">
-        <v>22648</v>
+        <v>22359</v>
       </c>
       <c r="K6" s="4">
         <f>IFERROR(((J6-J4)/J4*100),"")</f>
-        <v>0.19022340190223402</v>
-      </c>
-      <c r="L6"/>
+        <v>-0.20085698982324585</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
       <c r="M6" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N26" si="2">C6</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O6">
         <f t="shared" ref="O6:O26" si="3">D6</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="P6" s="1">
         <f>N6-O6</f>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="1">
         <f>R6-S6</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R6">
         <f t="shared" ref="R6:R26" si="4">H6</f>
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="S6">
         <f t="shared" ref="S6:S26" si="5">I6</f>
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="T6">
         <f t="shared" ref="T6:T26" si="6">J6</f>
-        <v>22648</v>
+        <v>22359</v>
       </c>
       <c r="U6" s="4">
         <f>((T6-T4)/T4*100)</f>
-        <v>0.19022340190223402</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
+        <v>-1.0882548108825481</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-1</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>22476</v>
+        <v>22400</v>
       </c>
       <c r="K7" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J7-J6)/J6*100)),"")</f>
-        <v>-0.75944895796538325</v>
-      </c>
-      <c r="L7"/>
+        <v>0.18337134934478286</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
       <c r="M7" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" ref="P7:P26" si="7">N7-O7</f>
-        <v>-9</v>
+        <v>-1</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" ref="Q7:Q26" si="8">R7-S7</f>
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="S7">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="T7">
         <f t="shared" si="6"/>
-        <v>22476</v>
+        <v>22400</v>
       </c>
       <c r="U7" s="4">
         <f>((T7-T6)/T6*100)</f>
-        <v>-0.75944895796538325</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+        <v>0.18337134934478286</v>
+      </c>
+      <c r="V7" s="13">
+        <v>0.42777777777777781</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -943,33 +973,35 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>22443</v>
+        <v>22450</v>
       </c>
       <c r="K8" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J8-J7)/J7*100)),"")</f>
-        <v>-0.14682327816337426</v>
-      </c>
-      <c r="L8"/>
+        <v>0.2232142857142857</v>
+      </c>
+      <c r="L8" t="s">
+        <v>35</v>
+      </c>
       <c r="M8" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="7"/>
@@ -977,316 +1009,357 @@
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="8"/>
-        <v>-20</v>
+        <v>2</v>
       </c>
       <c r="R8">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="S8">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="T8">
         <f t="shared" si="6"/>
-        <v>22443</v>
+        <v>22450</v>
       </c>
       <c r="U8" s="4">
         <f>((T8-T7)/T7*100)</f>
-        <v>-0.14682327816337426</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
+        <v>0.2232142857142857</v>
+      </c>
+      <c r="V8" s="13">
+        <v>0.45208333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
         <v>4</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-27</v>
+        <v>-1</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>-63</v>
+        <v>-2</v>
       </c>
       <c r="H9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I9">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="J9">
-        <v>22302</v>
+        <v>22469</v>
       </c>
       <c r="K9" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J9-J8)/J8*100)),"")</f>
-        <v>-0.62825825424408499</v>
-      </c>
-      <c r="L9"/>
+        <v>8.4632516703786187E-2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
       <c r="M9" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N9">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="P9" s="1">
         <f t="shared" si="7"/>
-        <v>-27</v>
+        <v>-1</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="8"/>
-        <v>-63</v>
+        <v>-2</v>
       </c>
       <c r="R9">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S9">
         <f t="shared" si="5"/>
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="T9">
         <f t="shared" si="6"/>
-        <v>22302</v>
+        <v>22469</v>
       </c>
       <c r="U9" s="4">
         <f>((T9-T8)/T8*100)</f>
-        <v>-0.62825825424408499</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="14">
+        <v>8.4632516703786187E-2</v>
+      </c>
+      <c r="V9" s="13">
+        <v>0.46736111111111112</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
         <v>5</v>
       </c>
       <c r="C10">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>-23</v>
+        <v>-1</v>
       </c>
       <c r="H10">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I10">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="J10">
-        <v>22302</v>
+        <v>22476</v>
       </c>
       <c r="K10" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J10-J9)/J9*100)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L10"/>
+        <v>3.1154034447460944E-2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>35</v>
+      </c>
       <c r="M10" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="8"/>
-        <v>-23</v>
+        <v>-1</v>
       </c>
       <c r="R10">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="S10">
         <f t="shared" si="5"/>
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="T10">
         <f t="shared" si="6"/>
-        <v>22302</v>
+        <v>22476</v>
       </c>
       <c r="U10" s="4">
         <f>((T10-T9)/T9*100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="14">
+        <v>3.1154034447460944E-2</v>
+      </c>
+      <c r="V10" s="13">
+        <v>0.57986111111111105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
         <v>6</v>
       </c>
       <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
         <v>9</v>
-      </c>
-      <c r="D11">
-        <v>47</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-38</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>-36</v>
+        <v>-2</v>
       </c>
       <c r="H11">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I11">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="J11">
-        <v>21957</v>
+        <v>22475</v>
       </c>
       <c r="K11" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J11-J10)/J10*100)),"")</f>
-        <v>-1.5469464622006994</v>
-      </c>
-      <c r="L11"/>
+        <v>-4.4491902473749777E-3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>35</v>
+      </c>
       <c r="M11" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="7"/>
-        <v>-38</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="8"/>
-        <v>-36</v>
+        <v>-2</v>
       </c>
       <c r="R11">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="S11">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="T11">
         <f t="shared" si="6"/>
-        <v>21957</v>
+        <v>22475</v>
       </c>
       <c r="U11" s="4">
         <f t="shared" ref="U11:U14" si="9">((T11-T10)/T10*100)</f>
-        <v>-1.5469464622006994</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="14">
+        <v>-4.4491902473749777E-3</v>
+      </c>
+      <c r="V11" s="13">
+        <v>0.59652777777777777</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
         <v>7</v>
       </c>
       <c r="C12">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D12">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>-15</v>
+        <v>8</v>
       </c>
       <c r="H12">
+        <v>29</v>
+      </c>
+      <c r="I12">
         <v>21</v>
       </c>
-      <c r="I12">
-        <v>36</v>
-      </c>
       <c r="J12" s="9">
-        <v>22055</v>
+        <v>22449</v>
       </c>
       <c r="K12" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J12-J11)/J11*100)),"")</f>
-        <v>0.4463269116910325</v>
-      </c>
-      <c r="L12"/>
+        <v>-0.11568409343715239</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
       <c r="M12" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="8"/>
-        <v>-15</v>
+        <v>8</v>
       </c>
       <c r="R12">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="S12">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="T12">
         <f t="shared" si="6"/>
-        <v>22055</v>
+        <v>22449</v>
       </c>
       <c r="U12" s="4">
         <f t="shared" si="9"/>
-        <v>0.4463269116910325</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="14">
+        <v>-0.11568409343715239</v>
+      </c>
+      <c r="V12" s="13">
+        <v>0.62986111111111109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
         <v>8</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>22474</v>
+      </c>
+      <c r="K13" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J13-J12)/J12*100)),"")</f>
-        <v/>
+        <v>0.11136353512405897</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="M13" s="8" t="e">
         <f>#REF!</f>
@@ -1294,52 +1367,73 @@
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>22474</v>
       </c>
       <c r="U13" s="4">
         <f t="shared" si="9"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="14">
+        <v>0.11136353512405897</v>
+      </c>
+      <c r="V13" s="13">
+        <v>0.6381944444444444</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
         <v>9</v>
+      </c>
+      <c r="C14">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>36</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="4" t="str">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>34</v>
+      </c>
+      <c r="I14">
+        <v>27</v>
+      </c>
+      <c r="J14">
+        <v>22466</v>
+      </c>
+      <c r="K14" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J14-J13)/J13*100)),"")</f>
-        <v/>
+        <v>-3.559668950787577E-2</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="M14" s="8" t="e">
         <f>#REF!</f>
@@ -1347,39 +1441,42 @@
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R14">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="S14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T14">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U14" s="4" t="e">
+        <v>22466</v>
+      </c>
+      <c r="U14" s="4">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="14">
+        <v>-3.559668950787577E-2</v>
+      </c>
+      <c r="V14" s="13">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
         <v>10</v>
       </c>
       <c r="E15" s="1">
@@ -1426,13 +1523,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U15" s="4" t="e">
+      <c r="U15" s="4">
         <f>(T15-T14)/T14*100</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="14">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
         <v>11</v>
       </c>
       <c r="E16" s="1">
@@ -1485,7 +1582,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>12</v>
       </c>
       <c r="E17" s="1">
@@ -1538,7 +1635,7 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>13</v>
       </c>
       <c r="E18" s="1">
@@ -1591,7 +1688,7 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="14">
+      <c r="B19" s="12">
         <v>14</v>
       </c>
       <c r="E19" s="1">
@@ -1644,7 +1741,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <v>15</v>
       </c>
       <c r="E20" s="1">
@@ -1697,7 +1794,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="14">
+      <c r="B21" s="12">
         <v>16</v>
       </c>
       <c r="E21" s="1">
@@ -1750,7 +1847,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="14">
+      <c r="B22" s="12">
         <v>17</v>
       </c>
       <c r="E22" s="1">
@@ -1803,7 +1900,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="14">
+      <c r="B23" s="12">
         <v>18</v>
       </c>
       <c r="E23" s="1">
@@ -1856,7 +1953,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="14">
+      <c r="B24" s="12">
         <v>19</v>
       </c>
       <c r="E24" s="1">
@@ -1905,7 +2002,7 @@
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="14">
+      <c r="B25" s="12">
         <v>20</v>
       </c>
       <c r="E25" s="1">
@@ -1954,7 +2051,7 @@
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
+      <c r="B26" s="12"/>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2513,34 +2610,34 @@
     <mergeCell ref="C3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="E6:E26">
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G26">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P26">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:Q26">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed Excel calling. Also added function to get excel results and filter them for bullish and bearish counts.
</commit_message>
<xml_diff>
--- a/Excels/IntradayTrend.xlsx
+++ b/Excels/IntradayTrend.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -140,16 +140,13 @@
     <t>S.No</t>
   </si>
   <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
     <t>NIFTY</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>ALL</t>
   </si>
 </sst>
 </file>
@@ -687,8 +684,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +738,7 @@
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="J4" s="10">
-        <v>22404</v>
+        <v>22967</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4"/>
@@ -779,7 +776,7 @@
         <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>0</v>
@@ -809,7 +806,7 @@
         <v>27</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
@@ -817,34 +814,34 @@
         <v>1</v>
       </c>
       <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
         <v>11</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E26" si="0">(C6-D6)</f>
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ref="G6:G26" si="1">H6-I6</f>
         <v>6</v>
       </c>
       <c r="H6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>22359</v>
+        <v>22972</v>
       </c>
       <c r="K6" s="4">
         <f>IFERROR(((J6-J4)/J4*100),"")</f>
-        <v>-0.20085698982324585</v>
+        <v>2.1770366177559106E-2</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M6" s="8" t="e">
         <f>#REF!</f>
@@ -852,15 +849,15 @@
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N26" si="2">C6</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="O6">
         <f t="shared" ref="O6:O26" si="3">D6</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P6" s="1">
         <f>N6-O6</f>
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="Q6" s="1">
         <f>R6-S6</f>
@@ -868,19 +865,22 @@
       </c>
       <c r="R6">
         <f t="shared" ref="R6:R26" si="4">H6</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S6">
         <f t="shared" ref="S6:S26" si="5">I6</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T6">
         <f t="shared" ref="T6:T26" si="6">J6</f>
-        <v>22359</v>
+        <v>22972</v>
       </c>
       <c r="U6" s="4">
         <f>((T6-T4)/T4*100)</f>
-        <v>-1.0882548108825481</v>
+        <v>1.6235346162353461</v>
+      </c>
+      <c r="V6" s="13">
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
@@ -888,592 +888,202 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>9</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J7">
-        <v>22400</v>
+        <v>23015</v>
       </c>
       <c r="K7" s="4">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J7-J6)/J6*100)),"")</f>
-        <v>0.18337134934478286</v>
+        <v>0.18718439839804979</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" ref="P7:P26" si="7">N7-O7</f>
-        <v>-1</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" ref="Q7:Q26" si="8">R7-S7</f>
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="6"/>
-        <v>22400</v>
-      </c>
-      <c r="U7" s="4">
-        <f>((T7-T6)/T6*100)</f>
-        <v>0.18337134934478286</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="U7" s="4"/>
       <c r="V7" s="13">
-        <v>0.42777777777777781</v>
+        <v>0.54652777777777783</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>22450</v>
-      </c>
-      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J8-J7)/J7*100)),"")</f>
-        <v>0.2232142857142857</v>
-      </c>
-      <c r="L8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="7"/>
-        <v>-3</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="6"/>
-        <v>22450</v>
-      </c>
-      <c r="U8" s="4">
-        <f>((T8-T7)/T7*100)</f>
-        <v>0.2232142857142857</v>
-      </c>
-      <c r="V8" s="13">
-        <v>0.45208333333333334</v>
-      </c>
+        <v/>
+      </c>
+      <c r="L8"/>
+      <c r="M8" s="8"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="13"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>4</v>
       </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9">
-        <v>22469</v>
-      </c>
-      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J9-J8)/J8*100)),"")</f>
-        <v>8.4632516703786187E-2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" si="7"/>
-        <v>-1</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" si="8"/>
-        <v>-2</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="6"/>
-        <v>22469</v>
-      </c>
-      <c r="U9" s="4">
-        <f>((T9-T8)/T8*100)</f>
-        <v>8.4632516703786187E-2</v>
-      </c>
-      <c r="V9" s="13">
-        <v>0.46736111111111112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="L9"/>
+      <c r="M9" s="8"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="13"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>22476</v>
-      </c>
-      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J10-J9)/J9*100)),"")</f>
-        <v>3.1154034447460944E-2</v>
-      </c>
-      <c r="L10" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="P10" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="6"/>
-        <v>22476</v>
-      </c>
-      <c r="U10" s="4">
-        <f>((T10-T9)/T9*100)</f>
-        <v>3.1154034447460944E-2</v>
-      </c>
-      <c r="V10" s="13">
-        <v>0.57986111111111105</v>
-      </c>
+        <v/>
+      </c>
+      <c r="L10"/>
+      <c r="M10" s="8"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="13"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>6</v>
       </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11">
-        <v>9</v>
-      </c>
-      <c r="J11">
-        <v>22475</v>
-      </c>
-      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J11-J10)/J10*100)),"")</f>
-        <v>-4.4491902473749777E-3</v>
-      </c>
-      <c r="L11" t="s">
-        <v>35</v>
-      </c>
-      <c r="M11" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="P11" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="8"/>
-        <v>-2</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="6"/>
-        <v>22475</v>
-      </c>
-      <c r="U11" s="4">
-        <f t="shared" ref="U11:U14" si="9">((T11-T10)/T10*100)</f>
-        <v>-4.4491902473749777E-3</v>
-      </c>
-      <c r="V11" s="13">
-        <v>0.59652777777777777</v>
-      </c>
+        <v/>
+      </c>
+      <c r="L11"/>
+      <c r="M11" s="8"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="13"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>7</v>
       </c>
-      <c r="C12">
-        <v>37</v>
-      </c>
-      <c r="D12">
-        <v>34</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H12">
-        <v>29</v>
-      </c>
-      <c r="I12">
-        <v>21</v>
-      </c>
-      <c r="J12" s="9">
-        <v>22449</v>
-      </c>
-      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J12-J11)/J11*100)),"")</f>
-        <v>-0.11568409343715239</v>
-      </c>
-      <c r="L12" t="s">
-        <v>38</v>
-      </c>
-      <c r="M12" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="P12" s="1">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="Q12" s="1">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="6"/>
-        <v>22449</v>
-      </c>
-      <c r="U12" s="4">
-        <f t="shared" si="9"/>
-        <v>-0.11568409343715239</v>
-      </c>
-      <c r="V12" s="13">
-        <v>0.62986111111111109</v>
-      </c>
+        <v/>
+      </c>
+      <c r="L12"/>
+      <c r="M12" s="8"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="13"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>8</v>
       </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>7</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
-      </c>
-      <c r="J13">
-        <v>22474</v>
-      </c>
-      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J13-J12)/J12*100)),"")</f>
-        <v>0.11136353512405897</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="6"/>
-        <v>22474</v>
-      </c>
-      <c r="U13" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11136353512405897</v>
-      </c>
-      <c r="V13" s="13">
-        <v>0.6381944444444444</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="13"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
         <v>9</v>
       </c>
-      <c r="C14">
-        <v>28</v>
-      </c>
-      <c r="D14">
-        <v>36</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="H14">
-        <v>34</v>
-      </c>
-      <c r="I14">
-        <v>27</v>
-      </c>
-      <c r="J14">
-        <v>22466</v>
-      </c>
-      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4" t="str">
         <f>IFERROR(IF(Table3[[#This Row],[NF Close]]="","",((J14-J13)/J13*100)),"")</f>
-        <v>-3.559668950787577E-2</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M14" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="P14" s="1">
-        <f t="shared" si="7"/>
-        <v>-8</v>
-      </c>
-      <c r="Q14" s="1">
-        <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="4"/>
-        <v>34</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="5"/>
-        <v>27</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="6"/>
-        <v>22466</v>
-      </c>
-      <c r="U14" s="4">
-        <f t="shared" si="9"/>
-        <v>-3.559668950787577E-2</v>
-      </c>
-      <c r="V14" s="13">
-        <v>0.65</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="13"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
@@ -1504,11 +1114,11 @@
         <v>0</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="P15:P26" si="7">N15-O15</f>
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="Q15:Q26" si="8">R15-S15</f>
         <v>0</v>
       </c>
       <c r="R15">
@@ -1523,9 +1133,9 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15" s="4" t="e">
         <f>(T15-T14)/T14*100</f>
-        <v>-100</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
@@ -1630,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="4" t="e">
-        <f t="shared" ref="U17:U23" si="10">(T17-T16)/T16*100</f>
+        <f t="shared" ref="U17:U23" si="9">(T17-T16)/T16*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1683,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="U18" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1736,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="U19" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1789,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1842,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="U21" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1895,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="U22" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1948,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="U23" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2164,7 +1774,7 @@
         <v>22338</v>
       </c>
       <c r="J55" s="4">
-        <f t="shared" ref="J55:J73" si="11">((I55-I54)/I54*100)</f>
+        <f t="shared" ref="J55:J73" si="10">((I55-I54)/I54*100)</f>
         <v>1.6148842287221945</v>
       </c>
     </row>
@@ -2188,7 +1798,7 @@
         <v>22378</v>
       </c>
       <c r="J56" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.17906706061420002</v>
       </c>
     </row>
@@ -2212,7 +1822,7 @@
         <v>22405</v>
       </c>
       <c r="J57" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.12065421396013941</v>
       </c>
     </row>
@@ -2236,7 +1846,7 @@
         <v>22356</v>
       </c>
       <c r="J58" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-0.21870118277170272</v>
       </c>
     </row>
@@ -2260,7 +1870,7 @@
         <v>22474</v>
       </c>
       <c r="J59" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.52782250849883694</v>
       </c>
     </row>
@@ -2284,7 +1894,7 @@
         <v>22493</v>
       </c>
       <c r="J60" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>8.4542137581204949E-2</v>
       </c>
     </row>
@@ -2308,7 +1918,7 @@
         <v>22332</v>
       </c>
       <c r="J61" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-0.71577824211977059</v>
       </c>
     </row>
@@ -2332,7 +1942,7 @@
         <v>22335</v>
       </c>
       <c r="J62" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.3433637829124127E-2</v>
       </c>
     </row>
@@ -2356,7 +1966,7 @@
         <v>21997</v>
       </c>
       <c r="J63" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-1.5133199014998882</v>
       </c>
     </row>
@@ -2380,7 +1990,7 @@
         <v>22146</v>
       </c>
       <c r="J64" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.67736509524026001</v>
       </c>
     </row>
@@ -2404,7 +2014,7 @@
         <v>22023</v>
       </c>
       <c r="J65" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-0.55540503928474672</v>
       </c>
     </row>
@@ -2428,7 +2038,7 @@
         <v>22055</v>
       </c>
       <c r="J66" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.14530263815102393</v>
       </c>
     </row>
@@ -2452,7 +2062,7 @@
         <v>21810</v>
       </c>
       <c r="J67" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-1.1108592155973702</v>
       </c>
     </row>
@@ -2476,7 +2086,7 @@
         <v>21839</v>
       </c>
       <c r="J68" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.13296652911508483</v>
       </c>
     </row>
@@ -2500,7 +2110,7 @@
         <v>22014</v>
       </c>
       <c r="J69" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.80131874170062733</v>
       </c>
     </row>
@@ -2524,7 +2134,7 @@
         <v>22096</v>
       </c>
       <c r="J70" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.37249023348778054</v>
       </c>
     </row>
@@ -2548,7 +2158,7 @@
         <v>22020</v>
       </c>
       <c r="J71" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-0.3439536567704562</v>
       </c>
     </row>
@@ -2572,7 +2182,7 @@
         <v>22147</v>
       </c>
       <c r="J72" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.57674841053587644</v>
       </c>
     </row>
@@ -2596,7 +2206,7 @@
         <v>22343</v>
       </c>
       <c r="J73" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.88499571047997472</v>
       </c>
     </row>

</xml_diff>